<commit_message>
Implementação de login inicial
</commit_message>
<xml_diff>
--- a/Agenda_Energisa.xlsx
+++ b/Agenda_Energisa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luciano\Desktop\Projeto Agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201F8456-09F3-42BA-A8F4-0E107476F2B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4704AF92-0161-436A-B7BA-26BAB3E5BAD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página2" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="137">
   <si>
     <t>Tarefa</t>
   </si>
@@ -429,6 +429,12 @@
   </si>
   <si>
     <t>trocar para um calendário que fique em portogues</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Fazer o compare para a senha e enviar a senha criptografada</t>
   </si>
 </sst>
 </file>
@@ -499,12 +505,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="27">
@@ -878,7 +890,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -988,10 +1000,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1003,14 +1020,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1279,7 +1293,7 @@
   </sheetPr>
   <dimension ref="A1:J297"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
@@ -1295,7 +1309,7 @@
     <col min="7" max="7" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1317,13 +1331,13 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="46"/>
-    </row>
-    <row r="2" spans="1:10" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="42"/>
+      <c r="J1" s="43"/>
+    </row>
+    <row r="2" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1341,11 +1355,11 @@
         <v>45469</v>
       </c>
       <c r="G2" s="9"/>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="43"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -1366,7 +1380,7 @@
       </c>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1385,7 +1399,7 @@
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
@@ -1404,7 +1418,7 @@
       </c>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -1423,7 +1437,7 @@
       </c>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -1442,7 +1456,7 @@
       </c>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -1461,7 +1475,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>16</v>
       </c>
@@ -1480,7 +1494,7 @@
       </c>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -1499,7 +1513,7 @@
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>19</v>
       </c>
@@ -1518,7 +1532,7 @@
       </c>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -1537,7 +1551,7 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>21</v>
       </c>
@@ -1556,7 +1570,7 @@
       </c>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -1575,7 +1589,7 @@
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>23</v>
       </c>
@@ -1594,7 +1608,7 @@
       </c>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
@@ -1613,7 +1627,7 @@
       </c>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
@@ -1632,7 +1646,7 @@
       </c>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>26</v>
       </c>
@@ -1651,7 +1665,7 @@
       </c>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>27</v>
       </c>
@@ -1666,7 +1680,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="15"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>28</v>
       </c>
@@ -1681,7 +1695,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>29</v>
       </c>
@@ -1696,7 +1710,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>30</v>
       </c>
@@ -1713,7 +1727,7 @@
       <c r="F22" s="21"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>31</v>
       </c>
@@ -1732,7 +1746,7 @@
       </c>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
@@ -1747,7 +1761,7 @@
       <c r="F24" s="21"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>35</v>
       </c>
@@ -1766,7 +1780,7 @@
       </c>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
@@ -1785,7 +1799,7 @@
       </c>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>37</v>
       </c>
@@ -1804,7 +1818,7 @@
       </c>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
@@ -1823,7 +1837,7 @@
       </c>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>39</v>
       </c>
@@ -1842,7 +1856,7 @@
       </c>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
@@ -1859,7 +1873,7 @@
       <c r="F30" s="21"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>42</v>
       </c>
@@ -1878,7 +1892,7 @@
       </c>
       <c r="G31" s="15"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>43</v>
       </c>
@@ -1897,7 +1911,7 @@
       </c>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>44</v>
       </c>
@@ -1916,7 +1930,7 @@
       </c>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>45</v>
       </c>
@@ -1935,7 +1949,7 @@
       </c>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>46</v>
       </c>
@@ -1954,7 +1968,7 @@
       </c>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>47</v>
       </c>
@@ -1969,7 +1983,7 @@
       <c r="F36" s="21"/>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>48</v>
       </c>
@@ -1988,7 +2002,7 @@
       </c>
       <c r="G37" s="15"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>49</v>
       </c>
@@ -2007,7 +2021,7 @@
       </c>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>50</v>
       </c>
@@ -2026,7 +2040,7 @@
       </c>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>51</v>
       </c>
@@ -2045,7 +2059,7 @@
       </c>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>52</v>
       </c>
@@ -2060,7 +2074,7 @@
       <c r="F41" s="19"/>
       <c r="G41" s="15"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>53</v>
       </c>
@@ -2073,7 +2087,7 @@
       <c r="F42" s="21"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>54</v>
       </c>
@@ -2086,7 +2100,7 @@
       <c r="F43" s="19"/>
       <c r="G43" s="15"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>55</v>
       </c>
@@ -2099,7 +2113,7 @@
       <c r="F44" s="21"/>
       <c r="G44" s="9"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>56</v>
       </c>
@@ -2118,7 +2132,7 @@
       </c>
       <c r="G45" s="15"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>57</v>
       </c>
@@ -2137,7 +2151,7 @@
       </c>
       <c r="G46" s="9"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>58</v>
       </c>
@@ -2156,7 +2170,7 @@
       </c>
       <c r="G47" s="15"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>59</v>
       </c>
@@ -2175,7 +2189,7 @@
       </c>
       <c r="G48" s="9"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>60</v>
       </c>
@@ -2194,7 +2208,7 @@
       </c>
       <c r="G49" s="15"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>61</v>
       </c>
@@ -2213,7 +2227,7 @@
       </c>
       <c r="G50" s="9"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>62</v>
       </c>
@@ -2232,7 +2246,7 @@
       </c>
       <c r="G51" s="15"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>63</v>
       </c>
@@ -2251,7 +2265,7 @@
       </c>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>64</v>
       </c>
@@ -2270,7 +2284,7 @@
       </c>
       <c r="G53" s="15"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>65</v>
       </c>
@@ -2289,7 +2303,7 @@
       </c>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>66</v>
       </c>
@@ -2308,7 +2322,7 @@
       </c>
       <c r="G55" s="15"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>67</v>
       </c>
@@ -2327,7 +2341,7 @@
       </c>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>68</v>
       </c>
@@ -2342,7 +2356,7 @@
       <c r="F57" s="19"/>
       <c r="G57" s="15"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>69</v>
       </c>
@@ -2357,7 +2371,7 @@
       <c r="F58" s="21"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>70</v>
       </c>
@@ -2372,7 +2386,7 @@
       <c r="F59" s="19"/>
       <c r="G59" s="15"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>71</v>
       </c>
@@ -2391,7 +2405,7 @@
       </c>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
         <v>72</v>
       </c>
@@ -2410,7 +2424,7 @@
       </c>
       <c r="G61" s="15"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>73</v>
       </c>
@@ -2429,7 +2443,7 @@
       </c>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
         <v>74</v>
       </c>
@@ -2448,7 +2462,7 @@
       </c>
       <c r="G63" s="15"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>75</v>
       </c>
@@ -2467,7 +2481,7 @@
       </c>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
         <v>76</v>
       </c>
@@ -2486,7 +2500,7 @@
       </c>
       <c r="G65" s="15"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>77</v>
       </c>
@@ -2505,7 +2519,7 @@
       </c>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>78</v>
       </c>
@@ -2524,7 +2538,7 @@
       </c>
       <c r="G67" s="15"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>79</v>
       </c>
@@ -2543,7 +2557,7 @@
       </c>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
         <v>80</v>
       </c>
@@ -2562,7 +2576,7 @@
       </c>
       <c r="G69" s="15"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>81</v>
       </c>
@@ -2581,7 +2595,7 @@
       </c>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
         <v>82</v>
       </c>
@@ -2600,7 +2614,7 @@
       </c>
       <c r="G71" s="15"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
         <v>83</v>
       </c>
@@ -2619,7 +2633,7 @@
       </c>
       <c r="G72" s="9"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
         <v>84</v>
       </c>
@@ -2638,7 +2652,7 @@
       </c>
       <c r="G73" s="15"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>85</v>
       </c>
@@ -2657,7 +2671,7 @@
       </c>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
         <v>86</v>
       </c>
@@ -2676,7 +2690,7 @@
       </c>
       <c r="G75" s="15"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>87</v>
       </c>
@@ -2695,7 +2709,7 @@
       </c>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
         <v>88</v>
       </c>
@@ -2714,7 +2728,7 @@
       </c>
       <c r="G77" s="15"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>89</v>
       </c>
@@ -2733,7 +2747,7 @@
       </c>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
         <v>90</v>
       </c>
@@ -2752,7 +2766,7 @@
       </c>
       <c r="G79" s="15"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="24" t="s">
         <v>91</v>
       </c>
@@ -2771,7 +2785,7 @@
       </c>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
         <v>92</v>
       </c>
@@ -2790,7 +2804,7 @@
       </c>
       <c r="G81" s="25"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>94</v>
       </c>
@@ -2807,7 +2821,7 @@
       <c r="F82" s="21"/>
       <c r="G82" s="26"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="17" t="s">
         <v>95</v>
       </c>
@@ -2824,7 +2838,7 @@
       <c r="F83" s="19"/>
       <c r="G83" s="25"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>96</v>
       </c>
@@ -2841,7 +2855,7 @@
       <c r="F84" s="21"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="17" t="s">
         <v>98</v>
       </c>
@@ -2856,7 +2870,7 @@
       <c r="F85" s="19"/>
       <c r="G85" s="15"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>99</v>
       </c>
@@ -2875,7 +2889,7 @@
       </c>
       <c r="G86" s="9"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
         <v>100</v>
       </c>
@@ -2888,7 +2902,7 @@
       <c r="F87" s="19"/>
       <c r="G87" s="15"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>101</v>
       </c>
@@ -2907,7 +2921,7 @@
       </c>
       <c r="G88" s="9"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
         <v>102</v>
       </c>
@@ -2926,7 +2940,7 @@
       </c>
       <c r="G89" s="15"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>103</v>
       </c>
@@ -2945,7 +2959,7 @@
       </c>
       <c r="G90" s="9"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
         <v>104</v>
       </c>
@@ -2964,7 +2978,7 @@
       </c>
       <c r="G91" s="15"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>105</v>
       </c>
@@ -2983,7 +2997,7 @@
       </c>
       <c r="G92" s="9"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
         <v>106</v>
       </c>
@@ -3002,7 +3016,7 @@
       </c>
       <c r="G93" s="15"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>107</v>
       </c>
@@ -3021,7 +3035,7 @@
       </c>
       <c r="G94" s="9"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
         <v>108</v>
       </c>
@@ -3040,7 +3054,7 @@
       </c>
       <c r="G95" s="15"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>109</v>
       </c>
@@ -3059,7 +3073,7 @@
       </c>
       <c r="G96" s="9"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
         <v>110</v>
       </c>
@@ -3078,7 +3092,7 @@
       </c>
       <c r="G97" s="25"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>111</v>
       </c>
@@ -3091,7 +3105,7 @@
       <c r="F98" s="21"/>
       <c r="G98" s="9"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
         <v>112</v>
       </c>
@@ -3104,7 +3118,7 @@
       <c r="F99" s="19"/>
       <c r="G99" s="15"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>113</v>
       </c>
@@ -3117,7 +3131,7 @@
       <c r="F100" s="21"/>
       <c r="G100" s="9"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
         <v>114</v>
       </c>
@@ -3130,7 +3144,7 @@
       <c r="F101" s="19"/>
       <c r="G101" s="15"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>115</v>
       </c>
@@ -3143,7 +3157,7 @@
       <c r="F102" s="21"/>
       <c r="G102" s="9"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="10"/>
       <c r="B103" s="11"/>
       <c r="C103" s="27"/>
@@ -3152,7 +3166,7 @@
       <c r="F103" s="19"/>
       <c r="G103" s="15"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
       <c r="B104" s="5"/>
       <c r="C104" s="22"/>
@@ -3161,7 +3175,7 @@
       <c r="F104" s="21"/>
       <c r="G104" s="9"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="10"/>
       <c r="B105" s="11"/>
       <c r="C105" s="27"/>
@@ -3170,7 +3184,7 @@
       <c r="F105" s="19"/>
       <c r="G105" s="15"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
       <c r="B106" s="5"/>
       <c r="C106" s="22"/>
@@ -3179,7 +3193,7 @@
       <c r="F106" s="21"/>
       <c r="G106" s="9"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="10"/>
       <c r="B107" s="11"/>
       <c r="C107" s="27"/>
@@ -3188,7 +3202,7 @@
       <c r="F107" s="19"/>
       <c r="G107" s="15"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
       <c r="B108" s="5"/>
       <c r="C108" s="22"/>
@@ -3197,7 +3211,7 @@
       <c r="F108" s="21"/>
       <c r="G108" s="9"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="10"/>
       <c r="B109" s="11"/>
       <c r="C109" s="27"/>
@@ -3206,7 +3220,7 @@
       <c r="F109" s="19"/>
       <c r="G109" s="15"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
       <c r="B110" s="5"/>
       <c r="C110" s="22"/>
@@ -3215,7 +3229,7 @@
       <c r="F110" s="21"/>
       <c r="G110" s="9"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="10"/>
       <c r="B111" s="11"/>
       <c r="C111" s="27"/>
@@ -3224,7 +3238,7 @@
       <c r="F111" s="19"/>
       <c r="G111" s="15"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
       <c r="B112" s="5"/>
       <c r="C112" s="22"/>
@@ -3233,7 +3247,7 @@
       <c r="F112" s="21"/>
       <c r="G112" s="9"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="10"/>
       <c r="B113" s="11"/>
       <c r="C113" s="27"/>
@@ -3242,7 +3256,7 @@
       <c r="F113" s="19"/>
       <c r="G113" s="15"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="4"/>
       <c r="B114" s="5"/>
       <c r="C114" s="22"/>
@@ -3251,7 +3265,7 @@
       <c r="F114" s="21"/>
       <c r="G114" s="9"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="10"/>
       <c r="B115" s="11"/>
       <c r="C115" s="27"/>
@@ -3260,7 +3274,7 @@
       <c r="F115" s="19"/>
       <c r="G115" s="15"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="4"/>
       <c r="B116" s="5"/>
       <c r="C116" s="22"/>
@@ -3269,7 +3283,7 @@
       <c r="F116" s="21"/>
       <c r="G116" s="9"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="10"/>
       <c r="B117" s="11"/>
       <c r="C117" s="27"/>
@@ -3278,7 +3292,7 @@
       <c r="F117" s="19"/>
       <c r="G117" s="15"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="4"/>
       <c r="B118" s="5"/>
       <c r="C118" s="22"/>
@@ -3287,7 +3301,7 @@
       <c r="F118" s="21"/>
       <c r="G118" s="9"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="10"/>
       <c r="B119" s="11"/>
       <c r="C119" s="27"/>
@@ -3296,7 +3310,7 @@
       <c r="F119" s="19"/>
       <c r="G119" s="15"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="4"/>
       <c r="B120" s="5"/>
       <c r="C120" s="22"/>
@@ -3305,7 +3319,7 @@
       <c r="F120" s="21"/>
       <c r="G120" s="9"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="10"/>
       <c r="B121" s="11"/>
       <c r="C121" s="27"/>
@@ -3314,7 +3328,7 @@
       <c r="F121" s="19"/>
       <c r="G121" s="15"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="4"/>
       <c r="B122" s="5"/>
       <c r="C122" s="22"/>
@@ -3323,7 +3337,7 @@
       <c r="F122" s="21"/>
       <c r="G122" s="9"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="10"/>
       <c r="B123" s="11"/>
       <c r="C123" s="27"/>
@@ -3332,7 +3346,7 @@
       <c r="F123" s="19"/>
       <c r="G123" s="15"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
       <c r="B124" s="5"/>
       <c r="C124" s="22"/>
@@ -3341,7 +3355,7 @@
       <c r="F124" s="21"/>
       <c r="G124" s="9"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="10"/>
       <c r="B125" s="11"/>
       <c r="C125" s="27"/>
@@ -3350,7 +3364,7 @@
       <c r="F125" s="19"/>
       <c r="G125" s="15"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
       <c r="B126" s="5"/>
       <c r="C126" s="22"/>
@@ -3359,7 +3373,7 @@
       <c r="F126" s="21"/>
       <c r="G126" s="9"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="10"/>
       <c r="B127" s="11"/>
       <c r="C127" s="27"/>
@@ -3368,7 +3382,7 @@
       <c r="F127" s="19"/>
       <c r="G127" s="15"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
       <c r="B128" s="5"/>
       <c r="C128" s="22"/>
@@ -3377,7 +3391,7 @@
       <c r="F128" s="21"/>
       <c r="G128" s="9"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="10"/>
       <c r="B129" s="11"/>
       <c r="C129" s="27"/>
@@ -3386,7 +3400,7 @@
       <c r="F129" s="19"/>
       <c r="G129" s="15"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="4"/>
       <c r="B130" s="5"/>
       <c r="C130" s="22"/>
@@ -3395,7 +3409,7 @@
       <c r="F130" s="21"/>
       <c r="G130" s="9"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="10"/>
       <c r="B131" s="11"/>
       <c r="C131" s="27"/>
@@ -3404,7 +3418,7 @@
       <c r="F131" s="19"/>
       <c r="G131" s="15"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="4"/>
       <c r="B132" s="5"/>
       <c r="C132" s="22"/>
@@ -3413,7 +3427,7 @@
       <c r="F132" s="21"/>
       <c r="G132" s="9"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="10"/>
       <c r="B133" s="11"/>
       <c r="C133" s="27"/>
@@ -3422,7 +3436,7 @@
       <c r="F133" s="19"/>
       <c r="G133" s="15"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
       <c r="B134" s="5"/>
       <c r="C134" s="22"/>
@@ -3431,7 +3445,7 @@
       <c r="F134" s="21"/>
       <c r="G134" s="9"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="10"/>
       <c r="B135" s="11"/>
       <c r="C135" s="27"/>
@@ -3440,7 +3454,7 @@
       <c r="F135" s="19"/>
       <c r="G135" s="15"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="4"/>
       <c r="B136" s="5"/>
       <c r="C136" s="22"/>
@@ -3449,7 +3463,7 @@
       <c r="F136" s="21"/>
       <c r="G136" s="9"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="10"/>
       <c r="B137" s="11"/>
       <c r="C137" s="27"/>
@@ -3458,7 +3472,7 @@
       <c r="F137" s="19"/>
       <c r="G137" s="15"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="4"/>
       <c r="B138" s="5"/>
       <c r="C138" s="22"/>
@@ -3467,7 +3481,7 @@
       <c r="F138" s="21"/>
       <c r="G138" s="9"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="10"/>
       <c r="B139" s="11"/>
       <c r="C139" s="27"/>
@@ -3476,7 +3490,7 @@
       <c r="F139" s="19"/>
       <c r="G139" s="15"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="4"/>
       <c r="B140" s="5"/>
       <c r="C140" s="22"/>
@@ -3485,7 +3499,7 @@
       <c r="F140" s="21"/>
       <c r="G140" s="9"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="10"/>
       <c r="B141" s="11"/>
       <c r="C141" s="27"/>
@@ -3494,7 +3508,7 @@
       <c r="F141" s="19"/>
       <c r="G141" s="15"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="4"/>
       <c r="B142" s="5"/>
       <c r="C142" s="22"/>
@@ -3503,7 +3517,7 @@
       <c r="F142" s="21"/>
       <c r="G142" s="9"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="10"/>
       <c r="B143" s="11"/>
       <c r="C143" s="27"/>
@@ -3512,7 +3526,7 @@
       <c r="F143" s="19"/>
       <c r="G143" s="15"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="4"/>
       <c r="B144" s="5"/>
       <c r="C144" s="22"/>
@@ -3521,7 +3535,7 @@
       <c r="F144" s="21"/>
       <c r="G144" s="9"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="10"/>
       <c r="B145" s="11"/>
       <c r="C145" s="27"/>
@@ -3530,7 +3544,7 @@
       <c r="F145" s="19"/>
       <c r="G145" s="15"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="4"/>
       <c r="B146" s="5"/>
       <c r="C146" s="22"/>
@@ -3539,7 +3553,7 @@
       <c r="F146" s="21"/>
       <c r="G146" s="9"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="10"/>
       <c r="B147" s="11"/>
       <c r="C147" s="27"/>
@@ -3548,7 +3562,7 @@
       <c r="F147" s="19"/>
       <c r="G147" s="15"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="4"/>
       <c r="B148" s="5"/>
       <c r="C148" s="22"/>
@@ -3557,7 +3571,7 @@
       <c r="F148" s="21"/>
       <c r="G148" s="9"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="10"/>
       <c r="B149" s="11"/>
       <c r="C149" s="27"/>
@@ -3566,7 +3580,7 @@
       <c r="F149" s="19"/>
       <c r="G149" s="15"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="4"/>
       <c r="B150" s="5"/>
       <c r="C150" s="22"/>
@@ -3575,7 +3589,7 @@
       <c r="F150" s="21"/>
       <c r="G150" s="9"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="10"/>
       <c r="B151" s="11"/>
       <c r="C151" s="27"/>
@@ -3584,7 +3598,7 @@
       <c r="F151" s="19"/>
       <c r="G151" s="15"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="4"/>
       <c r="B152" s="5"/>
       <c r="C152" s="22"/>
@@ -3593,7 +3607,7 @@
       <c r="F152" s="21"/>
       <c r="G152" s="9"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="10"/>
       <c r="B153" s="11"/>
       <c r="C153" s="27"/>
@@ -3602,7 +3616,7 @@
       <c r="F153" s="19"/>
       <c r="G153" s="15"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="4"/>
       <c r="B154" s="5"/>
       <c r="C154" s="22"/>
@@ -3611,7 +3625,7 @@
       <c r="F154" s="21"/>
       <c r="G154" s="9"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="10"/>
       <c r="B155" s="11"/>
       <c r="C155" s="27"/>
@@ -3620,7 +3634,7 @@
       <c r="F155" s="19"/>
       <c r="G155" s="15"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="4"/>
       <c r="B156" s="5"/>
       <c r="C156" s="22"/>
@@ -3629,7 +3643,7 @@
       <c r="F156" s="21"/>
       <c r="G156" s="9"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="10"/>
       <c r="B157" s="11"/>
       <c r="C157" s="27"/>
@@ -3638,7 +3652,7 @@
       <c r="F157" s="19"/>
       <c r="G157" s="15"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
       <c r="C158" s="22"/>
@@ -3647,7 +3661,7 @@
       <c r="F158" s="21"/>
       <c r="G158" s="9"/>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="10"/>
       <c r="B159" s="11"/>
       <c r="C159" s="27"/>
@@ -3656,7 +3670,7 @@
       <c r="F159" s="19"/>
       <c r="G159" s="15"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
       <c r="C160" s="22"/>
@@ -3665,7 +3679,7 @@
       <c r="F160" s="21"/>
       <c r="G160" s="9"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="10"/>
       <c r="B161" s="11"/>
       <c r="C161" s="27"/>
@@ -3674,7 +3688,7 @@
       <c r="F161" s="19"/>
       <c r="G161" s="15"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
       <c r="C162" s="22"/>
@@ -3683,7 +3697,7 @@
       <c r="F162" s="21"/>
       <c r="G162" s="9"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="10"/>
       <c r="B163" s="11"/>
       <c r="C163" s="27"/>
@@ -3692,7 +3706,7 @@
       <c r="F163" s="19"/>
       <c r="G163" s="15"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
       <c r="C164" s="22"/>
@@ -3701,7 +3715,7 @@
       <c r="F164" s="21"/>
       <c r="G164" s="9"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="10"/>
       <c r="B165" s="11"/>
       <c r="C165" s="27"/>
@@ -3710,7 +3724,7 @@
       <c r="F165" s="19"/>
       <c r="G165" s="15"/>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
       <c r="C166" s="22"/>
@@ -3719,7 +3733,7 @@
       <c r="F166" s="21"/>
       <c r="G166" s="9"/>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="10"/>
       <c r="B167" s="11"/>
       <c r="C167" s="27"/>
@@ -3728,7 +3742,7 @@
       <c r="F167" s="19"/>
       <c r="G167" s="15"/>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
       <c r="C168" s="22"/>
@@ -3737,7 +3751,7 @@
       <c r="F168" s="21"/>
       <c r="G168" s="9"/>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="10"/>
       <c r="B169" s="11"/>
       <c r="C169" s="27"/>
@@ -3746,7 +3760,7 @@
       <c r="F169" s="19"/>
       <c r="G169" s="15"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
       <c r="C170" s="22"/>
@@ -3755,7 +3769,7 @@
       <c r="F170" s="21"/>
       <c r="G170" s="9"/>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="10"/>
       <c r="B171" s="11"/>
       <c r="C171" s="27"/>
@@ -3764,7 +3778,7 @@
       <c r="F171" s="19"/>
       <c r="G171" s="15"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
       <c r="C172" s="22"/>
@@ -3773,7 +3787,7 @@
       <c r="F172" s="21"/>
       <c r="G172" s="9"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" s="10"/>
       <c r="B173" s="11"/>
       <c r="C173" s="27"/>
@@ -3782,7 +3796,7 @@
       <c r="F173" s="19"/>
       <c r="G173" s="15"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
       <c r="C174" s="22"/>
@@ -3791,7 +3805,7 @@
       <c r="F174" s="21"/>
       <c r="G174" s="9"/>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="10"/>
       <c r="B175" s="11"/>
       <c r="C175" s="27"/>
@@ -3800,7 +3814,7 @@
       <c r="F175" s="19"/>
       <c r="G175" s="15"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
       <c r="C176" s="22"/>
@@ -3809,7 +3823,7 @@
       <c r="F176" s="21"/>
       <c r="G176" s="9"/>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="10"/>
       <c r="B177" s="11"/>
       <c r="C177" s="27"/>
@@ -3818,7 +3832,7 @@
       <c r="F177" s="19"/>
       <c r="G177" s="15"/>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
       <c r="C178" s="22"/>
@@ -3827,7 +3841,7 @@
       <c r="F178" s="21"/>
       <c r="G178" s="9"/>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="10"/>
       <c r="B179" s="11"/>
       <c r="C179" s="27"/>
@@ -3836,7 +3850,7 @@
       <c r="F179" s="19"/>
       <c r="G179" s="15"/>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
       <c r="C180" s="22"/>
@@ -3845,7 +3859,7 @@
       <c r="F180" s="21"/>
       <c r="G180" s="9"/>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" s="10"/>
       <c r="B181" s="11"/>
       <c r="C181" s="27"/>
@@ -3854,7 +3868,7 @@
       <c r="F181" s="19"/>
       <c r="G181" s="15"/>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
       <c r="C182" s="22"/>
@@ -3863,7 +3877,7 @@
       <c r="F182" s="21"/>
       <c r="G182" s="9"/>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="10"/>
       <c r="B183" s="11"/>
       <c r="C183" s="27"/>
@@ -3872,7 +3886,7 @@
       <c r="F183" s="19"/>
       <c r="G183" s="15"/>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
       <c r="C184" s="22"/>
@@ -3881,7 +3895,7 @@
       <c r="F184" s="21"/>
       <c r="G184" s="9"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="10"/>
       <c r="B185" s="11"/>
       <c r="C185" s="27"/>
@@ -3890,7 +3904,7 @@
       <c r="F185" s="19"/>
       <c r="G185" s="15"/>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
       <c r="C186" s="22"/>
@@ -3899,7 +3913,7 @@
       <c r="F186" s="21"/>
       <c r="G186" s="9"/>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="10"/>
       <c r="B187" s="11"/>
       <c r="C187" s="27"/>
@@ -3908,7 +3922,7 @@
       <c r="F187" s="19"/>
       <c r="G187" s="15"/>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
       <c r="C188" s="22"/>
@@ -3917,7 +3931,7 @@
       <c r="F188" s="21"/>
       <c r="G188" s="9"/>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A189" s="10"/>
       <c r="B189" s="11"/>
       <c r="C189" s="27"/>
@@ -3926,7 +3940,7 @@
       <c r="F189" s="19"/>
       <c r="G189" s="15"/>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
       <c r="C190" s="22"/>
@@ -3935,7 +3949,7 @@
       <c r="F190" s="21"/>
       <c r="G190" s="9"/>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="10"/>
       <c r="B191" s="11"/>
       <c r="C191" s="27"/>
@@ -3944,7 +3958,7 @@
       <c r="F191" s="19"/>
       <c r="G191" s="15"/>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
       <c r="C192" s="22"/>
@@ -3953,7 +3967,7 @@
       <c r="F192" s="21"/>
       <c r="G192" s="9"/>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="10"/>
       <c r="B193" s="11"/>
       <c r="C193" s="27"/>
@@ -3962,7 +3976,7 @@
       <c r="F193" s="19"/>
       <c r="G193" s="15"/>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
       <c r="C194" s="22"/>
@@ -3971,7 +3985,7 @@
       <c r="F194" s="21"/>
       <c r="G194" s="9"/>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="10"/>
       <c r="B195" s="11"/>
       <c r="C195" s="27"/>
@@ -3980,7 +3994,7 @@
       <c r="F195" s="19"/>
       <c r="G195" s="15"/>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
       <c r="C196" s="22"/>
@@ -3989,7 +4003,7 @@
       <c r="F196" s="21"/>
       <c r="G196" s="9"/>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A197" s="10"/>
       <c r="B197" s="11"/>
       <c r="C197" s="27"/>
@@ -3998,7 +4012,7 @@
       <c r="F197" s="19"/>
       <c r="G197" s="15"/>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
       <c r="C198" s="22"/>
@@ -4007,7 +4021,7 @@
       <c r="F198" s="21"/>
       <c r="G198" s="9"/>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="10"/>
       <c r="B199" s="11"/>
       <c r="C199" s="27"/>
@@ -4016,7 +4030,7 @@
       <c r="F199" s="19"/>
       <c r="G199" s="15"/>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
       <c r="C200" s="22"/>
@@ -4025,7 +4039,7 @@
       <c r="F200" s="21"/>
       <c r="G200" s="9"/>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A201" s="10"/>
       <c r="B201" s="11"/>
       <c r="C201" s="27"/>
@@ -4034,7 +4048,7 @@
       <c r="F201" s="19"/>
       <c r="G201" s="15"/>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
       <c r="C202" s="22"/>
@@ -4043,7 +4057,7 @@
       <c r="F202" s="21"/>
       <c r="G202" s="9"/>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A203" s="10"/>
       <c r="B203" s="11"/>
       <c r="C203" s="27"/>
@@ -4052,7 +4066,7 @@
       <c r="F203" s="19"/>
       <c r="G203" s="15"/>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
       <c r="C204" s="22"/>
@@ -4061,7 +4075,7 @@
       <c r="F204" s="21"/>
       <c r="G204" s="9"/>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A205" s="10"/>
       <c r="B205" s="11"/>
       <c r="C205" s="27"/>
@@ -4070,7 +4084,7 @@
       <c r="F205" s="19"/>
       <c r="G205" s="15"/>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
       <c r="C206" s="22"/>
@@ -4079,7 +4093,7 @@
       <c r="F206" s="21"/>
       <c r="G206" s="9"/>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A207" s="10"/>
       <c r="B207" s="11"/>
       <c r="C207" s="27"/>
@@ -4088,7 +4102,7 @@
       <c r="F207" s="19"/>
       <c r="G207" s="15"/>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
       <c r="C208" s="22"/>
@@ -4097,7 +4111,7 @@
       <c r="F208" s="21"/>
       <c r="G208" s="9"/>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A209" s="10"/>
       <c r="B209" s="11"/>
       <c r="C209" s="27"/>
@@ -4106,7 +4120,7 @@
       <c r="F209" s="19"/>
       <c r="G209" s="15"/>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
       <c r="C210" s="22"/>
@@ -4115,7 +4129,7 @@
       <c r="F210" s="21"/>
       <c r="G210" s="9"/>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A211" s="10"/>
       <c r="B211" s="11"/>
       <c r="C211" s="27"/>
@@ -4124,7 +4138,7 @@
       <c r="F211" s="19"/>
       <c r="G211" s="15"/>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
       <c r="C212" s="22"/>
@@ -4133,7 +4147,7 @@
       <c r="F212" s="21"/>
       <c r="G212" s="9"/>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A213" s="10"/>
       <c r="B213" s="11"/>
       <c r="C213" s="27"/>
@@ -4142,7 +4156,7 @@
       <c r="F213" s="19"/>
       <c r="G213" s="15"/>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
       <c r="C214" s="22"/>
@@ -4151,7 +4165,7 @@
       <c r="F214" s="21"/>
       <c r="G214" s="9"/>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A215" s="10"/>
       <c r="B215" s="11"/>
       <c r="C215" s="27"/>
@@ -4160,7 +4174,7 @@
       <c r="F215" s="19"/>
       <c r="G215" s="15"/>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
       <c r="C216" s="22"/>
@@ -4169,7 +4183,7 @@
       <c r="F216" s="21"/>
       <c r="G216" s="9"/>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A217" s="10"/>
       <c r="B217" s="11"/>
       <c r="C217" s="27"/>
@@ -4178,7 +4192,7 @@
       <c r="F217" s="19"/>
       <c r="G217" s="15"/>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
       <c r="C218" s="22"/>
@@ -4187,7 +4201,7 @@
       <c r="F218" s="21"/>
       <c r="G218" s="9"/>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A219" s="10"/>
       <c r="B219" s="11"/>
       <c r="C219" s="27"/>
@@ -4196,7 +4210,7 @@
       <c r="F219" s="19"/>
       <c r="G219" s="15"/>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
       <c r="C220" s="22"/>
@@ -4205,7 +4219,7 @@
       <c r="F220" s="21"/>
       <c r="G220" s="9"/>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A221" s="10"/>
       <c r="B221" s="11"/>
       <c r="C221" s="27"/>
@@ -4214,7 +4228,7 @@
       <c r="F221" s="19"/>
       <c r="G221" s="15"/>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
       <c r="C222" s="22"/>
@@ -4223,7 +4237,7 @@
       <c r="F222" s="21"/>
       <c r="G222" s="9"/>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A223" s="10"/>
       <c r="B223" s="11"/>
       <c r="C223" s="27"/>
@@ -4232,7 +4246,7 @@
       <c r="F223" s="19"/>
       <c r="G223" s="15"/>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
       <c r="C224" s="22"/>
@@ -4241,7 +4255,7 @@
       <c r="F224" s="21"/>
       <c r="G224" s="9"/>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A225" s="10"/>
       <c r="B225" s="11"/>
       <c r="C225" s="27"/>
@@ -4250,7 +4264,7 @@
       <c r="F225" s="19"/>
       <c r="G225" s="15"/>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
       <c r="C226" s="22"/>
@@ -4259,7 +4273,7 @@
       <c r="F226" s="21"/>
       <c r="G226" s="9"/>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A227" s="10"/>
       <c r="B227" s="11"/>
       <c r="C227" s="27"/>
@@ -4268,7 +4282,7 @@
       <c r="F227" s="19"/>
       <c r="G227" s="15"/>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
       <c r="C228" s="22"/>
@@ -4277,7 +4291,7 @@
       <c r="F228" s="21"/>
       <c r="G228" s="9"/>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A229" s="10"/>
       <c r="B229" s="11"/>
       <c r="C229" s="27"/>
@@ -4286,7 +4300,7 @@
       <c r="F229" s="19"/>
       <c r="G229" s="15"/>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
       <c r="C230" s="22"/>
@@ -4295,7 +4309,7 @@
       <c r="F230" s="21"/>
       <c r="G230" s="9"/>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A231" s="10"/>
       <c r="B231" s="11"/>
       <c r="C231" s="27"/>
@@ -4304,7 +4318,7 @@
       <c r="F231" s="19"/>
       <c r="G231" s="15"/>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
       <c r="C232" s="22"/>
@@ -4313,7 +4327,7 @@
       <c r="F232" s="21"/>
       <c r="G232" s="9"/>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A233" s="10"/>
       <c r="B233" s="11"/>
       <c r="C233" s="27"/>
@@ -4322,7 +4336,7 @@
       <c r="F233" s="19"/>
       <c r="G233" s="15"/>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
       <c r="C234" s="22"/>
@@ -4331,7 +4345,7 @@
       <c r="F234" s="21"/>
       <c r="G234" s="9"/>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A235" s="10"/>
       <c r="B235" s="11"/>
       <c r="C235" s="27"/>
@@ -4340,7 +4354,7 @@
       <c r="F235" s="19"/>
       <c r="G235" s="15"/>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A236" s="4"/>
       <c r="B236" s="5"/>
       <c r="C236" s="22"/>
@@ -4349,7 +4363,7 @@
       <c r="F236" s="21"/>
       <c r="G236" s="9"/>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A237" s="10"/>
       <c r="B237" s="11"/>
       <c r="C237" s="27"/>
@@ -4358,7 +4372,7 @@
       <c r="F237" s="19"/>
       <c r="G237" s="15"/>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A238" s="4"/>
       <c r="B238" s="5"/>
       <c r="C238" s="22"/>
@@ -4367,7 +4381,7 @@
       <c r="F238" s="21"/>
       <c r="G238" s="9"/>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A239" s="10"/>
       <c r="B239" s="11"/>
       <c r="C239" s="27"/>
@@ -4376,7 +4390,7 @@
       <c r="F239" s="19"/>
       <c r="G239" s="15"/>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A240" s="4"/>
       <c r="B240" s="5"/>
       <c r="C240" s="22"/>
@@ -4385,7 +4399,7 @@
       <c r="F240" s="21"/>
       <c r="G240" s="9"/>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A241" s="10"/>
       <c r="B241" s="11"/>
       <c r="C241" s="27"/>
@@ -4394,7 +4408,7 @@
       <c r="F241" s="19"/>
       <c r="G241" s="15"/>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A242" s="4"/>
       <c r="B242" s="5"/>
       <c r="C242" s="22"/>
@@ -4403,7 +4417,7 @@
       <c r="F242" s="21"/>
       <c r="G242" s="9"/>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A243" s="10"/>
       <c r="B243" s="11"/>
       <c r="C243" s="27"/>
@@ -4412,7 +4426,7 @@
       <c r="F243" s="19"/>
       <c r="G243" s="15"/>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A244" s="4"/>
       <c r="B244" s="5"/>
       <c r="C244" s="22"/>
@@ -4421,7 +4435,7 @@
       <c r="F244" s="21"/>
       <c r="G244" s="9"/>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A245" s="10"/>
       <c r="B245" s="11"/>
       <c r="C245" s="27"/>
@@ -4430,7 +4444,7 @@
       <c r="F245" s="19"/>
       <c r="G245" s="15"/>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A246" s="4"/>
       <c r="B246" s="5"/>
       <c r="C246" s="22"/>
@@ -4439,7 +4453,7 @@
       <c r="F246" s="21"/>
       <c r="G246" s="9"/>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A247" s="10"/>
       <c r="B247" s="11"/>
       <c r="C247" s="27"/>
@@ -4448,7 +4462,7 @@
       <c r="F247" s="19"/>
       <c r="G247" s="15"/>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A248" s="4"/>
       <c r="B248" s="5"/>
       <c r="C248" s="22"/>
@@ -4457,7 +4471,7 @@
       <c r="F248" s="21"/>
       <c r="G248" s="9"/>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A249" s="10"/>
       <c r="B249" s="11"/>
       <c r="C249" s="27"/>
@@ -4466,7 +4480,7 @@
       <c r="F249" s="19"/>
       <c r="G249" s="15"/>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A250" s="4"/>
       <c r="B250" s="5"/>
       <c r="C250" s="22"/>
@@ -4475,7 +4489,7 @@
       <c r="F250" s="21"/>
       <c r="G250" s="9"/>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A251" s="10"/>
       <c r="B251" s="11"/>
       <c r="C251" s="27"/>
@@ -4484,7 +4498,7 @@
       <c r="F251" s="19"/>
       <c r="G251" s="15"/>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A252" s="4"/>
       <c r="B252" s="5"/>
       <c r="C252" s="22"/>
@@ -4493,7 +4507,7 @@
       <c r="F252" s="21"/>
       <c r="G252" s="9"/>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A253" s="10"/>
       <c r="B253" s="11"/>
       <c r="C253" s="27"/>
@@ -4502,7 +4516,7 @@
       <c r="F253" s="19"/>
       <c r="G253" s="15"/>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A254" s="4"/>
       <c r="B254" s="5"/>
       <c r="C254" s="22"/>
@@ -4511,7 +4525,7 @@
       <c r="F254" s="21"/>
       <c r="G254" s="9"/>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A255" s="10"/>
       <c r="B255" s="11"/>
       <c r="C255" s="27"/>
@@ -4520,7 +4534,7 @@
       <c r="F255" s="19"/>
       <c r="G255" s="15"/>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A256" s="4"/>
       <c r="B256" s="5"/>
       <c r="C256" s="22"/>
@@ -4529,7 +4543,7 @@
       <c r="F256" s="21"/>
       <c r="G256" s="9"/>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A257" s="10"/>
       <c r="B257" s="11"/>
       <c r="C257" s="27"/>
@@ -4538,7 +4552,7 @@
       <c r="F257" s="19"/>
       <c r="G257" s="15"/>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A258" s="4"/>
       <c r="B258" s="5"/>
       <c r="C258" s="22"/>
@@ -4547,7 +4561,7 @@
       <c r="F258" s="21"/>
       <c r="G258" s="9"/>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A259" s="10"/>
       <c r="B259" s="11"/>
       <c r="C259" s="27"/>
@@ -4556,7 +4570,7 @@
       <c r="F259" s="19"/>
       <c r="G259" s="15"/>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A260" s="4"/>
       <c r="B260" s="5"/>
       <c r="C260" s="22"/>
@@ -4565,7 +4579,7 @@
       <c r="F260" s="21"/>
       <c r="G260" s="9"/>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A261" s="10"/>
       <c r="B261" s="11"/>
       <c r="C261" s="27"/>
@@ -4574,7 +4588,7 @@
       <c r="F261" s="19"/>
       <c r="G261" s="15"/>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A262" s="4"/>
       <c r="B262" s="5"/>
       <c r="C262" s="22"/>
@@ -4583,7 +4597,7 @@
       <c r="F262" s="21"/>
       <c r="G262" s="9"/>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A263" s="10"/>
       <c r="B263" s="11"/>
       <c r="C263" s="27"/>
@@ -4592,7 +4606,7 @@
       <c r="F263" s="19"/>
       <c r="G263" s="15"/>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A264" s="4"/>
       <c r="B264" s="5"/>
       <c r="C264" s="22"/>
@@ -4601,7 +4615,7 @@
       <c r="F264" s="21"/>
       <c r="G264" s="9"/>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A265" s="10"/>
       <c r="B265" s="11"/>
       <c r="C265" s="27"/>
@@ -4610,7 +4624,7 @@
       <c r="F265" s="19"/>
       <c r="G265" s="15"/>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A266" s="4"/>
       <c r="B266" s="5"/>
       <c r="C266" s="22"/>
@@ -4619,7 +4633,7 @@
       <c r="F266" s="21"/>
       <c r="G266" s="9"/>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A267" s="10"/>
       <c r="B267" s="11"/>
       <c r="C267" s="27"/>
@@ -4628,7 +4642,7 @@
       <c r="F267" s="19"/>
       <c r="G267" s="15"/>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A268" s="4"/>
       <c r="B268" s="5"/>
       <c r="C268" s="22"/>
@@ -4637,7 +4651,7 @@
       <c r="F268" s="21"/>
       <c r="G268" s="9"/>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A269" s="10"/>
       <c r="B269" s="11"/>
       <c r="C269" s="27"/>
@@ -4646,7 +4660,7 @@
       <c r="F269" s="19"/>
       <c r="G269" s="15"/>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A270" s="4"/>
       <c r="B270" s="5"/>
       <c r="C270" s="22"/>
@@ -4655,7 +4669,7 @@
       <c r="F270" s="21"/>
       <c r="G270" s="9"/>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A271" s="10"/>
       <c r="B271" s="11"/>
       <c r="C271" s="27"/>
@@ -4664,7 +4678,7 @@
       <c r="F271" s="19"/>
       <c r="G271" s="15"/>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A272" s="4"/>
       <c r="B272" s="5"/>
       <c r="C272" s="22"/>
@@ -4673,7 +4687,7 @@
       <c r="F272" s="21"/>
       <c r="G272" s="9"/>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A273" s="10"/>
       <c r="B273" s="11"/>
       <c r="C273" s="27"/>
@@ -4682,7 +4696,7 @@
       <c r="F273" s="19"/>
       <c r="G273" s="15"/>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A274" s="4"/>
       <c r="B274" s="5"/>
       <c r="C274" s="22"/>
@@ -4691,7 +4705,7 @@
       <c r="F274" s="21"/>
       <c r="G274" s="9"/>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A275" s="10"/>
       <c r="B275" s="11"/>
       <c r="C275" s="27"/>
@@ -4700,7 +4714,7 @@
       <c r="F275" s="19"/>
       <c r="G275" s="15"/>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A276" s="4"/>
       <c r="B276" s="5"/>
       <c r="C276" s="22"/>
@@ -4709,7 +4723,7 @@
       <c r="F276" s="21"/>
       <c r="G276" s="9"/>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A277" s="10"/>
       <c r="B277" s="11"/>
       <c r="C277" s="27"/>
@@ -4718,7 +4732,7 @@
       <c r="F277" s="19"/>
       <c r="G277" s="15"/>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A278" s="4"/>
       <c r="B278" s="5"/>
       <c r="C278" s="22"/>
@@ -4727,7 +4741,7 @@
       <c r="F278" s="21"/>
       <c r="G278" s="9"/>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A279" s="10"/>
       <c r="B279" s="11"/>
       <c r="C279" s="27"/>
@@ -4736,7 +4750,7 @@
       <c r="F279" s="19"/>
       <c r="G279" s="15"/>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A280" s="4"/>
       <c r="B280" s="5"/>
       <c r="C280" s="22"/>
@@ -4745,7 +4759,7 @@
       <c r="F280" s="21"/>
       <c r="G280" s="9"/>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A281" s="10"/>
       <c r="B281" s="11"/>
       <c r="C281" s="27"/>
@@ -4754,7 +4768,7 @@
       <c r="F281" s="19"/>
       <c r="G281" s="15"/>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A282" s="4"/>
       <c r="B282" s="5"/>
       <c r="C282" s="22"/>
@@ -4763,7 +4777,7 @@
       <c r="F282" s="21"/>
       <c r="G282" s="9"/>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A283" s="10"/>
       <c r="B283" s="11"/>
       <c r="C283" s="27"/>
@@ -4772,7 +4786,7 @@
       <c r="F283" s="19"/>
       <c r="G283" s="15"/>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A284" s="4"/>
       <c r="B284" s="5"/>
       <c r="C284" s="22"/>
@@ -4781,7 +4795,7 @@
       <c r="F284" s="21"/>
       <c r="G284" s="9"/>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A285" s="10"/>
       <c r="B285" s="11"/>
       <c r="C285" s="27"/>
@@ -4790,7 +4804,7 @@
       <c r="F285" s="19"/>
       <c r="G285" s="15"/>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A286" s="4"/>
       <c r="B286" s="5"/>
       <c r="C286" s="22"/>
@@ -4799,7 +4813,7 @@
       <c r="F286" s="21"/>
       <c r="G286" s="9"/>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A287" s="10"/>
       <c r="B287" s="11"/>
       <c r="C287" s="27"/>
@@ -4808,7 +4822,7 @@
       <c r="F287" s="19"/>
       <c r="G287" s="15"/>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A288" s="4"/>
       <c r="B288" s="5"/>
       <c r="C288" s="22"/>
@@ -4817,7 +4831,7 @@
       <c r="F288" s="21"/>
       <c r="G288" s="9"/>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A289" s="10"/>
       <c r="B289" s="11"/>
       <c r="C289" s="27"/>
@@ -4826,7 +4840,7 @@
       <c r="F289" s="19"/>
       <c r="G289" s="15"/>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A290" s="4"/>
       <c r="B290" s="5"/>
       <c r="C290" s="22"/>
@@ -4835,7 +4849,7 @@
       <c r="F290" s="21"/>
       <c r="G290" s="9"/>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A291" s="10"/>
       <c r="B291" s="11"/>
       <c r="C291" s="27"/>
@@ -4844,7 +4858,7 @@
       <c r="F291" s="19"/>
       <c r="G291" s="15"/>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A292" s="4"/>
       <c r="B292" s="5"/>
       <c r="C292" s="22"/>
@@ -4853,7 +4867,7 @@
       <c r="F292" s="21"/>
       <c r="G292" s="9"/>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A293" s="10"/>
       <c r="B293" s="11"/>
       <c r="C293" s="27"/>
@@ -4862,7 +4876,7 @@
       <c r="F293" s="19"/>
       <c r="G293" s="15"/>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A294" s="4"/>
       <c r="B294" s="5"/>
       <c r="C294" s="22"/>
@@ -4871,7 +4885,7 @@
       <c r="F294" s="21"/>
       <c r="G294" s="9"/>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A295" s="10"/>
       <c r="B295" s="11"/>
       <c r="C295" s="27"/>
@@ -4880,7 +4894,7 @@
       <c r="F295" s="19"/>
       <c r="G295" s="15"/>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A296" s="4"/>
       <c r="B296" s="5"/>
       <c r="C296" s="22"/>
@@ -4889,7 +4903,7 @@
       <c r="F296" s="21"/>
       <c r="G296" s="9"/>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A297" s="28"/>
       <c r="B297" s="29"/>
       <c r="C297" s="30"/>
@@ -5021,10 +5035,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:D13"/>
+  <dimension ref="B1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B12:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5048,13 +5062,13 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="49">
         <v>38</v>
       </c>
     </row>
@@ -5129,36 +5143,50 @@
       </c>
       <c r="D10" s="33"/>
     </row>
-    <row r="11" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="47" t="s">
+    <row r="11" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="37" t="s">
         <v>134</v>
       </c>
       <c r="C11" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="44"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="33"/>
+    </row>
+    <row r="13" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="40"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
+    </row>
+    <row r="14" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="46"/>
-    </row>
-    <row r="13" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="41" t="s">
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
+    </row>
+    <row r="15" spans="2:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{CC114F35-AB6F-4605-B83C-47E18F7751EE}"/>
+    <hyperlink ref="B15" r:id="rId1" xr:uid="{CC114F35-AB6F-4605-B83C-47E18F7751EE}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>